<commit_message>
unit % to percent 1_0_yearly_rep.xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_0/1_0_yearly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_0/1_0_yearly_rep.xlsx
@@ -594,7 +594,7 @@
     <t xml:space="preserve">mrihff_</t>
   </si>
   <si>
-    <t xml:space="preserve">%</t>
+    <t xml:space="preserve">percent</t>
   </si>
   <si>
     <t xml:space="preserve">Repeated measures of child’s mean hepatic fat-fraction  measured using MRI: mrihff_: assessed within one year of childbirth (&gt;0 year and &lt;1 year) mrihff_1: assessed when the child was aged between bigger or equal to 1 year and &lt; 2 years … mrihff_17: assessed when the child was aged between bigger or equal to 17 years and &lt; 18 years</t>
@@ -867,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B52" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>